<commit_message>
fixed the date input error and added some descriptions to enter data in the preferred format
</commit_message>
<xml_diff>
--- a/general_use/SnowPit_data_entry_template.xlsx
+++ b/general_use/SnowPit_data_entry_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganmason/Documents/projects/lab_snowpits/general_use/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganmason/Documents/projects/lab_snowpits/snowpits/general_use/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925EF49A-41BC-F747-BD8C-D9FDC1D8BB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374F7FEB-80B4-9D42-89B8-842A57C7866E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="500" windowWidth="21420" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="500" windowWidth="30320" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="export" sheetId="1" r:id="rId1"/>
@@ -1698,11 +1698,230 @@
     <xf numFmtId="20" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1710,92 +1929,39 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1806,6 +1972,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1818,283 +1986,101 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2416,7 +2402,7 @@
   <dimension ref="A1:AE1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="U16" sqref="U16:U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2481,315 +2467,315 @@
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
-      <c r="B2" s="158" t="s">
+      <c r="B2" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="159" t="s">
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="160"/>
-      <c r="J2" s="161" t="s">
+      <c r="I2" s="135"/>
+      <c r="J2" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="92"/>
-      <c r="R2" s="92"/>
-      <c r="S2" s="92"/>
-      <c r="T2" s="92"/>
-      <c r="U2" s="92"/>
-      <c r="V2" s="162"/>
-      <c r="W2" s="150" t="s">
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+      <c r="O2" s="125"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="125"/>
+      <c r="R2" s="125"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="125"/>
+      <c r="V2" s="137"/>
+      <c r="W2" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="92"/>
-      <c r="Y2" s="92"/>
-      <c r="Z2" s="92"/>
-      <c r="AA2" s="92"/>
-      <c r="AB2" s="92"/>
-      <c r="AC2" s="92"/>
-      <c r="AD2" s="93"/>
+      <c r="X2" s="125"/>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="125"/>
+      <c r="AA2" s="125"/>
+      <c r="AB2" s="125"/>
+      <c r="AC2" s="125"/>
+      <c r="AD2" s="126"/>
       <c r="AE2" s="5"/>
     </row>
     <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
-      <c r="B3" s="163"/>
-      <c r="C3" s="218"/>
-      <c r="D3" s="218"/>
-      <c r="E3" s="218"/>
-      <c r="F3" s="218"/>
-      <c r="G3" s="219"/>
-      <c r="H3" s="164"/>
-      <c r="I3" s="219"/>
-      <c r="J3" s="165"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="135"/>
-      <c r="T3" s="136"/>
-      <c r="U3" s="166" t="s">
+      <c r="B3" s="138"/>
+      <c r="C3" s="139"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="98"/>
+      <c r="R3" s="98"/>
+      <c r="S3" s="98"/>
+      <c r="T3" s="106"/>
+      <c r="U3" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="136"/>
-      <c r="W3" s="151"/>
-      <c r="X3" s="135"/>
-      <c r="Y3" s="135"/>
-      <c r="Z3" s="135"/>
-      <c r="AA3" s="135"/>
-      <c r="AB3" s="135"/>
-      <c r="AC3" s="135"/>
-      <c r="AD3" s="144"/>
+      <c r="V3" s="106"/>
+      <c r="W3" s="127"/>
+      <c r="X3" s="98"/>
+      <c r="Y3" s="98"/>
+      <c r="Z3" s="98"/>
+      <c r="AA3" s="98"/>
+      <c r="AB3" s="98"/>
+      <c r="AC3" s="98"/>
+      <c r="AD3" s="99"/>
       <c r="AE3" s="6"/>
     </row>
     <row r="4" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="220"/>
-      <c r="C4" s="221"/>
-      <c r="D4" s="221"/>
-      <c r="E4" s="221"/>
-      <c r="F4" s="221"/>
-      <c r="G4" s="222"/>
-      <c r="H4" s="225"/>
-      <c r="I4" s="222"/>
-      <c r="J4" s="152"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="115"/>
-      <c r="U4" s="116"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="152"/>
-      <c r="X4" s="97"/>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="97"/>
-      <c r="AA4" s="97"/>
-      <c r="AB4" s="97"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="118"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="143"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="103"/>
+      <c r="Q4" s="103"/>
+      <c r="R4" s="103"/>
+      <c r="S4" s="103"/>
+      <c r="T4" s="104"/>
+      <c r="U4" s="96"/>
+      <c r="V4" s="94"/>
+      <c r="W4" s="111"/>
+      <c r="X4" s="103"/>
+      <c r="Y4" s="103"/>
+      <c r="Z4" s="103"/>
+      <c r="AA4" s="103"/>
+      <c r="AB4" s="103"/>
+      <c r="AC4" s="103"/>
+      <c r="AD4" s="128"/>
       <c r="AE4" s="6"/>
     </row>
     <row r="5" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
-      <c r="B5" s="156" t="s">
+      <c r="B5" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="157" t="s">
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="80"/>
-      <c r="J5" s="152"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="97"/>
-      <c r="O5" s="97"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="97"/>
-      <c r="R5" s="97"/>
-      <c r="S5" s="97"/>
-      <c r="T5" s="115"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="103"/>
+      <c r="S5" s="103"/>
+      <c r="T5" s="104"/>
       <c r="U5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="W5" s="152"/>
-      <c r="X5" s="97"/>
-      <c r="Y5" s="97"/>
-      <c r="Z5" s="97"/>
-      <c r="AA5" s="97"/>
-      <c r="AB5" s="97"/>
-      <c r="AC5" s="97"/>
-      <c r="AD5" s="118"/>
+      <c r="W5" s="111"/>
+      <c r="X5" s="103"/>
+      <c r="Y5" s="103"/>
+      <c r="Z5" s="103"/>
+      <c r="AA5" s="103"/>
+      <c r="AB5" s="103"/>
+      <c r="AC5" s="103"/>
+      <c r="AD5" s="128"/>
       <c r="AE5" s="6"/>
     </row>
     <row r="6" spans="1:31" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
-      <c r="B6" s="167"/>
-      <c r="C6" s="218"/>
-      <c r="D6" s="218"/>
-      <c r="E6" s="218"/>
-      <c r="F6" s="218"/>
-      <c r="G6" s="218"/>
-      <c r="H6" s="168"/>
-      <c r="I6" s="183"/>
-      <c r="J6" s="152"/>
-      <c r="K6" s="203"/>
-      <c r="L6" s="203"/>
-      <c r="M6" s="203"/>
-      <c r="N6" s="203"/>
-      <c r="O6" s="203"/>
-      <c r="P6" s="203"/>
-      <c r="Q6" s="203"/>
-      <c r="R6" s="203"/>
-      <c r="S6" s="203"/>
-      <c r="T6" s="115"/>
+      <c r="B6" s="149"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="139"/>
+      <c r="E6" s="139"/>
+      <c r="F6" s="139"/>
+      <c r="G6" s="139"/>
+      <c r="H6" s="150"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="147"/>
+      <c r="L6" s="147"/>
+      <c r="M6" s="147"/>
+      <c r="N6" s="147"/>
+      <c r="O6" s="147"/>
+      <c r="P6" s="147"/>
+      <c r="Q6" s="147"/>
+      <c r="R6" s="147"/>
+      <c r="S6" s="147"/>
+      <c r="T6" s="104"/>
       <c r="U6" s="77"/>
       <c r="V6" s="77"/>
-      <c r="W6" s="152"/>
-      <c r="X6" s="97"/>
-      <c r="Y6" s="97"/>
-      <c r="Z6" s="97"/>
-      <c r="AA6" s="97"/>
-      <c r="AB6" s="97"/>
-      <c r="AC6" s="97"/>
-      <c r="AD6" s="118"/>
+      <c r="W6" s="111"/>
+      <c r="X6" s="103"/>
+      <c r="Y6" s="103"/>
+      <c r="Z6" s="103"/>
+      <c r="AA6" s="103"/>
+      <c r="AB6" s="103"/>
+      <c r="AC6" s="103"/>
+      <c r="AD6" s="128"/>
       <c r="AE6" s="6"/>
     </row>
     <row r="7" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="166" t="s">
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
+      <c r="F7" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="101"/>
-      <c r="H7" s="166" t="s">
+      <c r="G7" s="152"/>
+      <c r="H7" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="100"/>
-      <c r="J7" s="227" t="s">
+      <c r="I7" s="153"/>
+      <c r="J7" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="K7" s="227"/>
-      <c r="L7" s="227"/>
-      <c r="M7" s="227"/>
-      <c r="N7" s="227" t="s">
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="O7" s="227"/>
-      <c r="P7" s="227"/>
-      <c r="Q7" s="227"/>
-      <c r="R7" s="227"/>
-      <c r="S7" s="228" t="s">
+      <c r="O7" s="92"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="92"/>
+      <c r="R7" s="92"/>
+      <c r="S7" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="T7" s="229"/>
-      <c r="U7" s="226" t="s">
+      <c r="T7" s="89"/>
+      <c r="U7" s="154" t="s">
         <v>12</v>
       </c>
-      <c r="V7" s="183"/>
-      <c r="W7" s="152"/>
-      <c r="X7" s="97"/>
-      <c r="Y7" s="97"/>
-      <c r="Z7" s="97"/>
-      <c r="AA7" s="97"/>
-      <c r="AB7" s="97"/>
-      <c r="AC7" s="97"/>
-      <c r="AD7" s="118"/>
+      <c r="V7" s="151"/>
+      <c r="W7" s="111"/>
+      <c r="X7" s="103"/>
+      <c r="Y7" s="103"/>
+      <c r="Z7" s="103"/>
+      <c r="AA7" s="103"/>
+      <c r="AB7" s="103"/>
+      <c r="AC7" s="103"/>
+      <c r="AD7" s="128"/>
       <c r="AE7" s="6"/>
     </row>
     <row r="8" spans="1:31" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="170"/>
-      <c r="C8" s="223"/>
-      <c r="D8" s="223"/>
-      <c r="E8" s="223"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="224"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="224"/>
-      <c r="J8" s="230"/>
-      <c r="K8" s="232"/>
-      <c r="L8" s="232"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="234"/>
-      <c r="O8" s="232"/>
-      <c r="P8" s="232"/>
-      <c r="Q8" s="232"/>
-      <c r="R8" s="232"/>
-      <c r="S8" s="234"/>
-      <c r="T8" s="232"/>
-      <c r="U8" s="231"/>
-      <c r="V8" s="235"/>
-      <c r="W8" s="153"/>
-      <c r="X8" s="88"/>
-      <c r="Y8" s="88"/>
-      <c r="Z8" s="88"/>
-      <c r="AA8" s="88"/>
-      <c r="AB8" s="88"/>
-      <c r="AC8" s="88"/>
-      <c r="AD8" s="154"/>
+      <c r="B8" s="156"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="157"/>
+      <c r="E8" s="157"/>
+      <c r="F8" s="158"/>
+      <c r="G8" s="159"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="159"/>
+      <c r="J8" s="164"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
+      <c r="M8" s="165"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="91"/>
+      <c r="P8" s="91"/>
+      <c r="Q8" s="91"/>
+      <c r="R8" s="91"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="91"/>
+      <c r="U8" s="161"/>
+      <c r="V8" s="162"/>
+      <c r="W8" s="115"/>
+      <c r="X8" s="116"/>
+      <c r="Y8" s="116"/>
+      <c r="Z8" s="116"/>
+      <c r="AA8" s="116"/>
+      <c r="AB8" s="116"/>
+      <c r="AC8" s="116"/>
+      <c r="AD8" s="122"/>
       <c r="AE8" s="6"/>
     </row>
     <row r="9" spans="1:31" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="228" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="94" t="s">
+      <c r="C9" s="125"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="125"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="229" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="93"/>
-      <c r="J9" s="95" t="s">
+      <c r="I9" s="126"/>
+      <c r="J9" s="230" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="93"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="141" t="s">
+      <c r="K9" s="126"/>
+      <c r="L9" s="231"/>
+      <c r="M9" s="163" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="92"/>
-      <c r="O9" s="92"/>
-      <c r="P9" s="92"/>
-      <c r="Q9" s="92"/>
-      <c r="R9" s="92"/>
-      <c r="S9" s="92"/>
-      <c r="T9" s="92"/>
-      <c r="U9" s="92"/>
-      <c r="V9" s="92"/>
-      <c r="W9" s="92"/>
-      <c r="X9" s="92"/>
-      <c r="Y9" s="92"/>
-      <c r="Z9" s="92"/>
-      <c r="AA9" s="92"/>
-      <c r="AB9" s="92"/>
-      <c r="AC9" s="92"/>
-      <c r="AD9" s="93"/>
+      <c r="N9" s="125"/>
+      <c r="O9" s="125"/>
+      <c r="P9" s="125"/>
+      <c r="Q9" s="125"/>
+      <c r="R9" s="125"/>
+      <c r="S9" s="125"/>
+      <c r="T9" s="125"/>
+      <c r="U9" s="125"/>
+      <c r="V9" s="125"/>
+      <c r="W9" s="125"/>
+      <c r="X9" s="125"/>
+      <c r="Y9" s="125"/>
+      <c r="Z9" s="125"/>
+      <c r="AA9" s="125"/>
+      <c r="AB9" s="125"/>
+      <c r="AC9" s="125"/>
+      <c r="AD9" s="126"/>
       <c r="AE9" s="8"/>
     </row>
     <row r="10" spans="1:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="80"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="94"/>
       <c r="E10" s="10" t="s">
         <v>18</v>
       </c>
@@ -2811,37 +2797,37 @@
       <c r="K10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="97"/>
-      <c r="M10" s="145" t="s">
+      <c r="L10" s="103"/>
+      <c r="M10" s="166" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="100"/>
-      <c r="O10" s="101"/>
-      <c r="P10" s="146" t="s">
+      <c r="N10" s="153"/>
+      <c r="O10" s="152"/>
+      <c r="P10" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="97"/>
-      <c r="R10" s="97"/>
-      <c r="S10" s="97"/>
-      <c r="T10" s="115"/>
-      <c r="U10" s="147" t="s">
+      <c r="Q10" s="103"/>
+      <c r="R10" s="103"/>
+      <c r="S10" s="103"/>
+      <c r="T10" s="104"/>
+      <c r="U10" s="168" t="s">
         <v>27</v>
       </c>
-      <c r="V10" s="148" t="s">
+      <c r="V10" s="169" t="s">
         <v>28</v>
       </c>
-      <c r="W10" s="147" t="s">
+      <c r="W10" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="X10" s="155" t="s">
+      <c r="X10" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="Y10" s="97"/>
-      <c r="Z10" s="97"/>
-      <c r="AA10" s="97"/>
-      <c r="AB10" s="97"/>
-      <c r="AC10" s="97"/>
-      <c r="AD10" s="118"/>
+      <c r="Y10" s="103"/>
+      <c r="Z10" s="103"/>
+      <c r="AA10" s="103"/>
+      <c r="AB10" s="103"/>
+      <c r="AC10" s="103"/>
+      <c r="AD10" s="128"/>
       <c r="AE10" s="15"/>
     </row>
     <row r="11" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2876,7 +2862,7 @@
       <c r="K11" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="97"/>
+      <c r="L11" s="103"/>
       <c r="M11" s="14" t="s">
         <v>31</v>
       </c>
@@ -2886,21 +2872,21 @@
       <c r="O11" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="P11" s="116"/>
-      <c r="Q11" s="79"/>
-      <c r="R11" s="79"/>
-      <c r="S11" s="79"/>
-      <c r="T11" s="80"/>
-      <c r="U11" s="142"/>
-      <c r="V11" s="80"/>
-      <c r="W11" s="142"/>
-      <c r="X11" s="79"/>
-      <c r="Y11" s="79"/>
-      <c r="Z11" s="79"/>
-      <c r="AA11" s="79"/>
-      <c r="AB11" s="79"/>
-      <c r="AC11" s="79"/>
-      <c r="AD11" s="119"/>
+      <c r="P11" s="96"/>
+      <c r="Q11" s="100"/>
+      <c r="R11" s="100"/>
+      <c r="S11" s="100"/>
+      <c r="T11" s="94"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="94"/>
+      <c r="W11" s="107"/>
+      <c r="X11" s="100"/>
+      <c r="Y11" s="100"/>
+      <c r="Z11" s="100"/>
+      <c r="AA11" s="100"/>
+      <c r="AB11" s="100"/>
+      <c r="AC11" s="100"/>
+      <c r="AD11" s="101"/>
       <c r="AE11" s="15"/>
     </row>
     <row r="12" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2917,27 +2903,27 @@
       <c r="I12" s="29"/>
       <c r="J12" s="30"/>
       <c r="K12" s="31"/>
-      <c r="L12" s="97"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="83" t="s">
+      <c r="L12" s="103"/>
+      <c r="M12" s="170"/>
+      <c r="N12" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="84"/>
-      <c r="P12" s="182"/>
-      <c r="Q12" s="97"/>
-      <c r="R12" s="97"/>
-      <c r="S12" s="97"/>
-      <c r="T12" s="115"/>
-      <c r="U12" s="134"/>
-      <c r="V12" s="84"/>
-      <c r="W12" s="149"/>
-      <c r="X12" s="143"/>
-      <c r="Y12" s="135"/>
-      <c r="Z12" s="135"/>
-      <c r="AA12" s="135"/>
-      <c r="AB12" s="135"/>
-      <c r="AC12" s="135"/>
-      <c r="AD12" s="144"/>
+      <c r="O12" s="93"/>
+      <c r="P12" s="102"/>
+      <c r="Q12" s="103"/>
+      <c r="R12" s="103"/>
+      <c r="S12" s="103"/>
+      <c r="T12" s="104"/>
+      <c r="U12" s="105"/>
+      <c r="V12" s="93"/>
+      <c r="W12" s="95"/>
+      <c r="X12" s="97"/>
+      <c r="Y12" s="98"/>
+      <c r="Z12" s="98"/>
+      <c r="AA12" s="98"/>
+      <c r="AB12" s="98"/>
+      <c r="AC12" s="98"/>
+      <c r="AD12" s="99"/>
       <c r="AE12" s="34"/>
     </row>
     <row r="13" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2954,25 +2940,25 @@
       <c r="I13" s="29"/>
       <c r="J13" s="35"/>
       <c r="K13" s="36"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="116"/>
-      <c r="Q13" s="79"/>
-      <c r="R13" s="79"/>
-      <c r="S13" s="79"/>
-      <c r="T13" s="80"/>
-      <c r="U13" s="142"/>
-      <c r="V13" s="80"/>
-      <c r="W13" s="116"/>
-      <c r="X13" s="116"/>
-      <c r="Y13" s="79"/>
-      <c r="Z13" s="79"/>
-      <c r="AA13" s="79"/>
-      <c r="AB13" s="79"/>
-      <c r="AC13" s="79"/>
-      <c r="AD13" s="119"/>
+      <c r="L13" s="103"/>
+      <c r="M13" s="171"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="94"/>
+      <c r="P13" s="96"/>
+      <c r="Q13" s="100"/>
+      <c r="R13" s="100"/>
+      <c r="S13" s="100"/>
+      <c r="T13" s="94"/>
+      <c r="U13" s="107"/>
+      <c r="V13" s="94"/>
+      <c r="W13" s="96"/>
+      <c r="X13" s="96"/>
+      <c r="Y13" s="100"/>
+      <c r="Z13" s="100"/>
+      <c r="AA13" s="100"/>
+      <c r="AB13" s="100"/>
+      <c r="AC13" s="100"/>
+      <c r="AD13" s="101"/>
       <c r="AE13" s="34"/>
     </row>
     <row r="14" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2989,27 +2975,27 @@
       <c r="I14" s="29"/>
       <c r="J14" s="35"/>
       <c r="K14" s="37"/>
-      <c r="L14" s="97"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="83" t="s">
+      <c r="L14" s="103"/>
+      <c r="M14" s="170"/>
+      <c r="N14" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="84"/>
-      <c r="P14" s="134"/>
-      <c r="Q14" s="135"/>
-      <c r="R14" s="135"/>
-      <c r="S14" s="135"/>
-      <c r="T14" s="136"/>
-      <c r="U14" s="134"/>
-      <c r="V14" s="84"/>
-      <c r="W14" s="149"/>
-      <c r="X14" s="143"/>
-      <c r="Y14" s="135"/>
-      <c r="Z14" s="135"/>
-      <c r="AA14" s="135"/>
-      <c r="AB14" s="135"/>
-      <c r="AC14" s="135"/>
-      <c r="AD14" s="144"/>
+      <c r="O14" s="93"/>
+      <c r="P14" s="105"/>
+      <c r="Q14" s="98"/>
+      <c r="R14" s="98"/>
+      <c r="S14" s="98"/>
+      <c r="T14" s="106"/>
+      <c r="U14" s="105"/>
+      <c r="V14" s="93"/>
+      <c r="W14" s="95"/>
+      <c r="X14" s="97"/>
+      <c r="Y14" s="98"/>
+      <c r="Z14" s="98"/>
+      <c r="AA14" s="98"/>
+      <c r="AB14" s="98"/>
+      <c r="AC14" s="98"/>
+      <c r="AD14" s="99"/>
       <c r="AE14" s="34"/>
     </row>
     <row r="15" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3026,25 +3012,25 @@
       <c r="I15" s="29"/>
       <c r="J15" s="38"/>
       <c r="K15" s="31"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="82"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="80"/>
-      <c r="P15" s="116"/>
-      <c r="Q15" s="79"/>
-      <c r="R15" s="79"/>
-      <c r="S15" s="79"/>
-      <c r="T15" s="80"/>
-      <c r="U15" s="142"/>
-      <c r="V15" s="80"/>
-      <c r="W15" s="116"/>
-      <c r="X15" s="116"/>
-      <c r="Y15" s="79"/>
-      <c r="Z15" s="79"/>
-      <c r="AA15" s="79"/>
-      <c r="AB15" s="79"/>
-      <c r="AC15" s="79"/>
-      <c r="AD15" s="119"/>
+      <c r="L15" s="103"/>
+      <c r="M15" s="171"/>
+      <c r="N15" s="100"/>
+      <c r="O15" s="94"/>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="100"/>
+      <c r="R15" s="100"/>
+      <c r="S15" s="100"/>
+      <c r="T15" s="94"/>
+      <c r="U15" s="107"/>
+      <c r="V15" s="94"/>
+      <c r="W15" s="96"/>
+      <c r="X15" s="96"/>
+      <c r="Y15" s="100"/>
+      <c r="Z15" s="100"/>
+      <c r="AA15" s="100"/>
+      <c r="AB15" s="100"/>
+      <c r="AC15" s="100"/>
+      <c r="AD15" s="101"/>
       <c r="AE15" s="34"/>
     </row>
     <row r="16" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3061,27 +3047,27 @@
       <c r="I16" s="29"/>
       <c r="J16" s="30"/>
       <c r="K16" s="31"/>
-      <c r="L16" s="97"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="83" t="s">
+      <c r="L16" s="103"/>
+      <c r="M16" s="170"/>
+      <c r="N16" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O16" s="84"/>
-      <c r="P16" s="134"/>
-      <c r="Q16" s="135"/>
-      <c r="R16" s="135"/>
-      <c r="S16" s="135"/>
-      <c r="T16" s="136"/>
-      <c r="U16" s="134"/>
-      <c r="V16" s="84"/>
-      <c r="W16" s="149"/>
-      <c r="X16" s="143"/>
-      <c r="Y16" s="135"/>
-      <c r="Z16" s="135"/>
-      <c r="AA16" s="135"/>
-      <c r="AB16" s="135"/>
-      <c r="AC16" s="135"/>
-      <c r="AD16" s="144"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="105"/>
+      <c r="Q16" s="98"/>
+      <c r="R16" s="98"/>
+      <c r="S16" s="98"/>
+      <c r="T16" s="106"/>
+      <c r="U16" s="105"/>
+      <c r="V16" s="93"/>
+      <c r="W16" s="95"/>
+      <c r="X16" s="97"/>
+      <c r="Y16" s="98"/>
+      <c r="Z16" s="98"/>
+      <c r="AA16" s="98"/>
+      <c r="AB16" s="98"/>
+      <c r="AC16" s="98"/>
+      <c r="AD16" s="99"/>
       <c r="AE16" s="34"/>
     </row>
     <row r="17" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3098,25 +3084,25 @@
       <c r="I17" s="29"/>
       <c r="J17" s="35"/>
       <c r="K17" s="39"/>
-      <c r="L17" s="97"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="80"/>
-      <c r="P17" s="116"/>
-      <c r="Q17" s="79"/>
-      <c r="R17" s="79"/>
-      <c r="S17" s="79"/>
-      <c r="T17" s="80"/>
-      <c r="U17" s="142"/>
-      <c r="V17" s="80"/>
-      <c r="W17" s="116"/>
-      <c r="X17" s="116"/>
-      <c r="Y17" s="79"/>
-      <c r="Z17" s="79"/>
-      <c r="AA17" s="79"/>
-      <c r="AB17" s="79"/>
-      <c r="AC17" s="79"/>
-      <c r="AD17" s="119"/>
+      <c r="L17" s="103"/>
+      <c r="M17" s="171"/>
+      <c r="N17" s="100"/>
+      <c r="O17" s="94"/>
+      <c r="P17" s="96"/>
+      <c r="Q17" s="100"/>
+      <c r="R17" s="100"/>
+      <c r="S17" s="100"/>
+      <c r="T17" s="94"/>
+      <c r="U17" s="107"/>
+      <c r="V17" s="94"/>
+      <c r="W17" s="96"/>
+      <c r="X17" s="96"/>
+      <c r="Y17" s="100"/>
+      <c r="Z17" s="100"/>
+      <c r="AA17" s="100"/>
+      <c r="AB17" s="100"/>
+      <c r="AC17" s="100"/>
+      <c r="AD17" s="101"/>
       <c r="AE17" s="34"/>
     </row>
     <row r="18" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3133,27 +3119,27 @@
       <c r="I18" s="29"/>
       <c r="J18" s="30"/>
       <c r="K18" s="31"/>
-      <c r="L18" s="97"/>
-      <c r="M18" s="81"/>
-      <c r="N18" s="83" t="s">
+      <c r="L18" s="103"/>
+      <c r="M18" s="170"/>
+      <c r="N18" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O18" s="84"/>
-      <c r="P18" s="134"/>
-      <c r="Q18" s="135"/>
-      <c r="R18" s="135"/>
-      <c r="S18" s="135"/>
-      <c r="T18" s="136"/>
-      <c r="U18" s="134"/>
-      <c r="V18" s="84"/>
-      <c r="W18" s="149"/>
-      <c r="X18" s="143"/>
-      <c r="Y18" s="135"/>
-      <c r="Z18" s="135"/>
-      <c r="AA18" s="135"/>
-      <c r="AB18" s="135"/>
-      <c r="AC18" s="135"/>
-      <c r="AD18" s="144"/>
+      <c r="O18" s="93"/>
+      <c r="P18" s="105"/>
+      <c r="Q18" s="98"/>
+      <c r="R18" s="98"/>
+      <c r="S18" s="98"/>
+      <c r="T18" s="106"/>
+      <c r="U18" s="105"/>
+      <c r="V18" s="93"/>
+      <c r="W18" s="95"/>
+      <c r="X18" s="97"/>
+      <c r="Y18" s="98"/>
+      <c r="Z18" s="98"/>
+      <c r="AA18" s="98"/>
+      <c r="AB18" s="98"/>
+      <c r="AC18" s="98"/>
+      <c r="AD18" s="99"/>
       <c r="AE18" s="34"/>
     </row>
     <row r="19" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3170,25 +3156,25 @@
       <c r="I19" s="29"/>
       <c r="J19" s="35"/>
       <c r="K19" s="39"/>
-      <c r="L19" s="97"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="116"/>
-      <c r="Q19" s="79"/>
-      <c r="R19" s="79"/>
-      <c r="S19" s="79"/>
-      <c r="T19" s="80"/>
-      <c r="U19" s="142"/>
-      <c r="V19" s="80"/>
-      <c r="W19" s="116"/>
-      <c r="X19" s="116"/>
-      <c r="Y19" s="79"/>
-      <c r="Z19" s="79"/>
-      <c r="AA19" s="79"/>
-      <c r="AB19" s="79"/>
-      <c r="AC19" s="79"/>
-      <c r="AD19" s="119"/>
+      <c r="L19" s="103"/>
+      <c r="M19" s="171"/>
+      <c r="N19" s="100"/>
+      <c r="O19" s="94"/>
+      <c r="P19" s="96"/>
+      <c r="Q19" s="100"/>
+      <c r="R19" s="100"/>
+      <c r="S19" s="100"/>
+      <c r="T19" s="94"/>
+      <c r="U19" s="107"/>
+      <c r="V19" s="94"/>
+      <c r="W19" s="96"/>
+      <c r="X19" s="96"/>
+      <c r="Y19" s="100"/>
+      <c r="Z19" s="100"/>
+      <c r="AA19" s="100"/>
+      <c r="AB19" s="100"/>
+      <c r="AC19" s="100"/>
+      <c r="AD19" s="101"/>
       <c r="AE19" s="34"/>
     </row>
     <row r="20" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3205,27 +3191,27 @@
       <c r="I20" s="29"/>
       <c r="J20" s="35"/>
       <c r="K20" s="29"/>
-      <c r="L20" s="97"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="83" t="s">
+      <c r="L20" s="103"/>
+      <c r="M20" s="170"/>
+      <c r="N20" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O20" s="84"/>
-      <c r="P20" s="134"/>
-      <c r="Q20" s="135"/>
-      <c r="R20" s="135"/>
-      <c r="S20" s="135"/>
-      <c r="T20" s="136"/>
-      <c r="U20" s="134"/>
-      <c r="V20" s="84"/>
-      <c r="W20" s="149"/>
-      <c r="X20" s="143"/>
-      <c r="Y20" s="135"/>
-      <c r="Z20" s="135"/>
-      <c r="AA20" s="135"/>
-      <c r="AB20" s="135"/>
-      <c r="AC20" s="135"/>
-      <c r="AD20" s="144"/>
+      <c r="O20" s="93"/>
+      <c r="P20" s="105"/>
+      <c r="Q20" s="98"/>
+      <c r="R20" s="98"/>
+      <c r="S20" s="98"/>
+      <c r="T20" s="106"/>
+      <c r="U20" s="105"/>
+      <c r="V20" s="93"/>
+      <c r="W20" s="95"/>
+      <c r="X20" s="97"/>
+      <c r="Y20" s="98"/>
+      <c r="Z20" s="98"/>
+      <c r="AA20" s="98"/>
+      <c r="AB20" s="98"/>
+      <c r="AC20" s="98"/>
+      <c r="AD20" s="99"/>
       <c r="AE20" s="34"/>
     </row>
     <row r="21" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3242,25 +3228,25 @@
       <c r="I21" s="29"/>
       <c r="J21" s="38"/>
       <c r="K21" s="39"/>
-      <c r="L21" s="97"/>
-      <c r="M21" s="82"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="80"/>
-      <c r="P21" s="116"/>
-      <c r="Q21" s="79"/>
-      <c r="R21" s="79"/>
-      <c r="S21" s="79"/>
-      <c r="T21" s="80"/>
-      <c r="U21" s="142"/>
-      <c r="V21" s="80"/>
-      <c r="W21" s="116"/>
-      <c r="X21" s="116"/>
-      <c r="Y21" s="79"/>
-      <c r="Z21" s="79"/>
-      <c r="AA21" s="79"/>
-      <c r="AB21" s="79"/>
-      <c r="AC21" s="79"/>
-      <c r="AD21" s="119"/>
+      <c r="L21" s="103"/>
+      <c r="M21" s="171"/>
+      <c r="N21" s="100"/>
+      <c r="O21" s="94"/>
+      <c r="P21" s="96"/>
+      <c r="Q21" s="100"/>
+      <c r="R21" s="100"/>
+      <c r="S21" s="100"/>
+      <c r="T21" s="94"/>
+      <c r="U21" s="107"/>
+      <c r="V21" s="94"/>
+      <c r="W21" s="96"/>
+      <c r="X21" s="96"/>
+      <c r="Y21" s="100"/>
+      <c r="Z21" s="100"/>
+      <c r="AA21" s="100"/>
+      <c r="AB21" s="100"/>
+      <c r="AC21" s="100"/>
+      <c r="AD21" s="101"/>
       <c r="AE21" s="34"/>
     </row>
     <row r="22" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3277,27 +3263,27 @@
       <c r="I22" s="29"/>
       <c r="J22" s="35"/>
       <c r="K22" s="29"/>
-      <c r="L22" s="97"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="83" t="s">
+      <c r="L22" s="103"/>
+      <c r="M22" s="170"/>
+      <c r="N22" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O22" s="84"/>
-      <c r="P22" s="134"/>
-      <c r="Q22" s="135"/>
-      <c r="R22" s="135"/>
-      <c r="S22" s="135"/>
-      <c r="T22" s="136"/>
-      <c r="U22" s="134"/>
-      <c r="V22" s="84"/>
-      <c r="W22" s="179"/>
-      <c r="X22" s="180"/>
-      <c r="Y22" s="135"/>
-      <c r="Z22" s="135"/>
-      <c r="AA22" s="135"/>
-      <c r="AB22" s="135"/>
-      <c r="AC22" s="135"/>
-      <c r="AD22" s="144"/>
+      <c r="O22" s="93"/>
+      <c r="P22" s="105"/>
+      <c r="Q22" s="98"/>
+      <c r="R22" s="98"/>
+      <c r="S22" s="98"/>
+      <c r="T22" s="106"/>
+      <c r="U22" s="105"/>
+      <c r="V22" s="93"/>
+      <c r="W22" s="108"/>
+      <c r="X22" s="109"/>
+      <c r="Y22" s="98"/>
+      <c r="Z22" s="98"/>
+      <c r="AA22" s="98"/>
+      <c r="AB22" s="98"/>
+      <c r="AC22" s="98"/>
+      <c r="AD22" s="99"/>
       <c r="AE22" s="34"/>
     </row>
     <row r="23" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3314,25 +3300,25 @@
       <c r="I23" s="29"/>
       <c r="J23" s="38"/>
       <c r="K23" s="39"/>
-      <c r="L23" s="97"/>
-      <c r="M23" s="82"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="80"/>
-      <c r="P23" s="116"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="79"/>
-      <c r="S23" s="79"/>
-      <c r="T23" s="80"/>
-      <c r="U23" s="142"/>
-      <c r="V23" s="80"/>
-      <c r="W23" s="142"/>
-      <c r="X23" s="79"/>
-      <c r="Y23" s="79"/>
-      <c r="Z23" s="79"/>
-      <c r="AA23" s="79"/>
-      <c r="AB23" s="79"/>
-      <c r="AC23" s="79"/>
-      <c r="AD23" s="119"/>
+      <c r="L23" s="103"/>
+      <c r="M23" s="171"/>
+      <c r="N23" s="100"/>
+      <c r="O23" s="94"/>
+      <c r="P23" s="96"/>
+      <c r="Q23" s="100"/>
+      <c r="R23" s="100"/>
+      <c r="S23" s="100"/>
+      <c r="T23" s="94"/>
+      <c r="U23" s="107"/>
+      <c r="V23" s="94"/>
+      <c r="W23" s="107"/>
+      <c r="X23" s="100"/>
+      <c r="Y23" s="100"/>
+      <c r="Z23" s="100"/>
+      <c r="AA23" s="100"/>
+      <c r="AB23" s="100"/>
+      <c r="AC23" s="100"/>
+      <c r="AD23" s="101"/>
       <c r="AE23" s="34"/>
     </row>
     <row r="24" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3349,27 +3335,27 @@
       <c r="I24" s="29"/>
       <c r="J24" s="35"/>
       <c r="K24" s="29"/>
-      <c r="L24" s="97"/>
-      <c r="M24" s="81"/>
-      <c r="N24" s="83" t="s">
+      <c r="L24" s="103"/>
+      <c r="M24" s="170"/>
+      <c r="N24" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O24" s="84"/>
-      <c r="P24" s="134"/>
-      <c r="Q24" s="135"/>
-      <c r="R24" s="135"/>
-      <c r="S24" s="135"/>
-      <c r="T24" s="136"/>
-      <c r="U24" s="134"/>
-      <c r="V24" s="84"/>
-      <c r="W24" s="179"/>
-      <c r="X24" s="180"/>
-      <c r="Y24" s="135"/>
-      <c r="Z24" s="135"/>
-      <c r="AA24" s="135"/>
-      <c r="AB24" s="135"/>
-      <c r="AC24" s="135"/>
-      <c r="AD24" s="144"/>
+      <c r="O24" s="93"/>
+      <c r="P24" s="105"/>
+      <c r="Q24" s="98"/>
+      <c r="R24" s="98"/>
+      <c r="S24" s="98"/>
+      <c r="T24" s="106"/>
+      <c r="U24" s="105"/>
+      <c r="V24" s="93"/>
+      <c r="W24" s="108"/>
+      <c r="X24" s="109"/>
+      <c r="Y24" s="98"/>
+      <c r="Z24" s="98"/>
+      <c r="AA24" s="98"/>
+      <c r="AB24" s="98"/>
+      <c r="AC24" s="98"/>
+      <c r="AD24" s="99"/>
       <c r="AE24" s="34"/>
     </row>
     <row r="25" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3386,25 +3372,25 @@
       <c r="I25" s="29"/>
       <c r="J25" s="38"/>
       <c r="K25" s="39"/>
-      <c r="L25" s="97"/>
-      <c r="M25" s="82"/>
-      <c r="N25" s="79"/>
-      <c r="O25" s="80"/>
-      <c r="P25" s="116"/>
-      <c r="Q25" s="79"/>
-      <c r="R25" s="79"/>
-      <c r="S25" s="79"/>
-      <c r="T25" s="80"/>
-      <c r="U25" s="142"/>
-      <c r="V25" s="80"/>
-      <c r="W25" s="142"/>
-      <c r="X25" s="79"/>
-      <c r="Y25" s="79"/>
-      <c r="Z25" s="79"/>
-      <c r="AA25" s="79"/>
-      <c r="AB25" s="79"/>
-      <c r="AC25" s="79"/>
-      <c r="AD25" s="119"/>
+      <c r="L25" s="103"/>
+      <c r="M25" s="171"/>
+      <c r="N25" s="100"/>
+      <c r="O25" s="94"/>
+      <c r="P25" s="96"/>
+      <c r="Q25" s="100"/>
+      <c r="R25" s="100"/>
+      <c r="S25" s="100"/>
+      <c r="T25" s="94"/>
+      <c r="U25" s="107"/>
+      <c r="V25" s="94"/>
+      <c r="W25" s="107"/>
+      <c r="X25" s="100"/>
+      <c r="Y25" s="100"/>
+      <c r="Z25" s="100"/>
+      <c r="AA25" s="100"/>
+      <c r="AB25" s="100"/>
+      <c r="AC25" s="100"/>
+      <c r="AD25" s="101"/>
       <c r="AE25" s="34"/>
     </row>
     <row r="26" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3421,27 +3407,27 @@
       <c r="I26" s="29"/>
       <c r="J26" s="35"/>
       <c r="K26" s="29"/>
-      <c r="L26" s="97"/>
-      <c r="M26" s="81"/>
-      <c r="N26" s="83" t="s">
+      <c r="L26" s="103"/>
+      <c r="M26" s="170"/>
+      <c r="N26" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O26" s="84"/>
-      <c r="P26" s="134"/>
-      <c r="Q26" s="135"/>
-      <c r="R26" s="135"/>
-      <c r="S26" s="135"/>
-      <c r="T26" s="136"/>
-      <c r="U26" s="134"/>
-      <c r="V26" s="84"/>
-      <c r="W26" s="179"/>
-      <c r="X26" s="180"/>
-      <c r="Y26" s="135"/>
-      <c r="Z26" s="135"/>
-      <c r="AA26" s="135"/>
-      <c r="AB26" s="135"/>
-      <c r="AC26" s="135"/>
-      <c r="AD26" s="144"/>
+      <c r="O26" s="93"/>
+      <c r="P26" s="105"/>
+      <c r="Q26" s="98"/>
+      <c r="R26" s="98"/>
+      <c r="S26" s="98"/>
+      <c r="T26" s="106"/>
+      <c r="U26" s="105"/>
+      <c r="V26" s="93"/>
+      <c r="W26" s="108"/>
+      <c r="X26" s="109"/>
+      <c r="Y26" s="98"/>
+      <c r="Z26" s="98"/>
+      <c r="AA26" s="98"/>
+      <c r="AB26" s="98"/>
+      <c r="AC26" s="98"/>
+      <c r="AD26" s="99"/>
       <c r="AE26" s="34"/>
     </row>
     <row r="27" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3458,25 +3444,25 @@
       <c r="I27" s="29"/>
       <c r="J27" s="38"/>
       <c r="K27" s="39"/>
-      <c r="L27" s="97"/>
-      <c r="M27" s="82"/>
-      <c r="N27" s="79"/>
-      <c r="O27" s="80"/>
-      <c r="P27" s="116"/>
-      <c r="Q27" s="79"/>
-      <c r="R27" s="79"/>
-      <c r="S27" s="79"/>
-      <c r="T27" s="80"/>
-      <c r="U27" s="142"/>
-      <c r="V27" s="80"/>
-      <c r="W27" s="142"/>
-      <c r="X27" s="79"/>
-      <c r="Y27" s="79"/>
-      <c r="Z27" s="79"/>
-      <c r="AA27" s="79"/>
-      <c r="AB27" s="79"/>
-      <c r="AC27" s="79"/>
-      <c r="AD27" s="119"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="171"/>
+      <c r="N27" s="100"/>
+      <c r="O27" s="94"/>
+      <c r="P27" s="96"/>
+      <c r="Q27" s="100"/>
+      <c r="R27" s="100"/>
+      <c r="S27" s="100"/>
+      <c r="T27" s="94"/>
+      <c r="U27" s="107"/>
+      <c r="V27" s="94"/>
+      <c r="W27" s="107"/>
+      <c r="X27" s="100"/>
+      <c r="Y27" s="100"/>
+      <c r="Z27" s="100"/>
+      <c r="AA27" s="100"/>
+      <c r="AB27" s="100"/>
+      <c r="AC27" s="100"/>
+      <c r="AD27" s="101"/>
       <c r="AE27" s="34"/>
     </row>
     <row r="28" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3493,27 +3479,27 @@
       <c r="I28" s="29"/>
       <c r="J28" s="35"/>
       <c r="K28" s="29"/>
-      <c r="L28" s="97"/>
-      <c r="M28" s="81"/>
-      <c r="N28" s="83" t="s">
+      <c r="L28" s="103"/>
+      <c r="M28" s="170"/>
+      <c r="N28" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O28" s="84"/>
-      <c r="P28" s="178"/>
-      <c r="Q28" s="135"/>
-      <c r="R28" s="135"/>
-      <c r="S28" s="135"/>
-      <c r="T28" s="136"/>
-      <c r="U28" s="134"/>
-      <c r="V28" s="84"/>
-      <c r="W28" s="179"/>
-      <c r="X28" s="180"/>
-      <c r="Y28" s="135"/>
-      <c r="Z28" s="135"/>
-      <c r="AA28" s="135"/>
-      <c r="AB28" s="135"/>
-      <c r="AC28" s="135"/>
-      <c r="AD28" s="144"/>
+      <c r="O28" s="93"/>
+      <c r="P28" s="110"/>
+      <c r="Q28" s="98"/>
+      <c r="R28" s="98"/>
+      <c r="S28" s="98"/>
+      <c r="T28" s="106"/>
+      <c r="U28" s="105"/>
+      <c r="V28" s="93"/>
+      <c r="W28" s="108"/>
+      <c r="X28" s="109"/>
+      <c r="Y28" s="98"/>
+      <c r="Z28" s="98"/>
+      <c r="AA28" s="98"/>
+      <c r="AB28" s="98"/>
+      <c r="AC28" s="98"/>
+      <c r="AD28" s="99"/>
       <c r="AE28" s="34"/>
     </row>
     <row r="29" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3530,25 +3516,25 @@
       <c r="I29" s="29"/>
       <c r="J29" s="38"/>
       <c r="K29" s="39"/>
-      <c r="L29" s="97"/>
-      <c r="M29" s="82"/>
-      <c r="N29" s="79"/>
-      <c r="O29" s="80"/>
-      <c r="P29" s="152"/>
-      <c r="Q29" s="97"/>
-      <c r="R29" s="97"/>
-      <c r="S29" s="97"/>
-      <c r="T29" s="115"/>
-      <c r="U29" s="142"/>
-      <c r="V29" s="80"/>
-      <c r="W29" s="142"/>
-      <c r="X29" s="79"/>
-      <c r="Y29" s="79"/>
-      <c r="Z29" s="79"/>
-      <c r="AA29" s="79"/>
-      <c r="AB29" s="79"/>
-      <c r="AC29" s="79"/>
-      <c r="AD29" s="119"/>
+      <c r="L29" s="103"/>
+      <c r="M29" s="171"/>
+      <c r="N29" s="100"/>
+      <c r="O29" s="94"/>
+      <c r="P29" s="111"/>
+      <c r="Q29" s="103"/>
+      <c r="R29" s="103"/>
+      <c r="S29" s="103"/>
+      <c r="T29" s="104"/>
+      <c r="U29" s="107"/>
+      <c r="V29" s="94"/>
+      <c r="W29" s="107"/>
+      <c r="X29" s="100"/>
+      <c r="Y29" s="100"/>
+      <c r="Z29" s="100"/>
+      <c r="AA29" s="100"/>
+      <c r="AB29" s="100"/>
+      <c r="AC29" s="100"/>
+      <c r="AD29" s="101"/>
       <c r="AE29" s="34"/>
     </row>
     <row r="30" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3565,27 +3551,27 @@
       <c r="I30" s="29"/>
       <c r="J30" s="35"/>
       <c r="K30" s="29"/>
-      <c r="L30" s="97"/>
-      <c r="M30" s="81"/>
-      <c r="N30" s="83" t="s">
+      <c r="L30" s="103"/>
+      <c r="M30" s="170"/>
+      <c r="N30" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O30" s="84"/>
-      <c r="P30" s="178"/>
-      <c r="Q30" s="135"/>
-      <c r="R30" s="135"/>
-      <c r="S30" s="135"/>
-      <c r="T30" s="136"/>
-      <c r="U30" s="134"/>
-      <c r="V30" s="84"/>
-      <c r="W30" s="179"/>
-      <c r="X30" s="180"/>
-      <c r="Y30" s="135"/>
-      <c r="Z30" s="135"/>
-      <c r="AA30" s="135"/>
-      <c r="AB30" s="135"/>
-      <c r="AC30" s="135"/>
-      <c r="AD30" s="144"/>
+      <c r="O30" s="93"/>
+      <c r="P30" s="110"/>
+      <c r="Q30" s="98"/>
+      <c r="R30" s="98"/>
+      <c r="S30" s="98"/>
+      <c r="T30" s="106"/>
+      <c r="U30" s="105"/>
+      <c r="V30" s="93"/>
+      <c r="W30" s="108"/>
+      <c r="X30" s="109"/>
+      <c r="Y30" s="98"/>
+      <c r="Z30" s="98"/>
+      <c r="AA30" s="98"/>
+      <c r="AB30" s="98"/>
+      <c r="AC30" s="98"/>
+      <c r="AD30" s="99"/>
       <c r="AE30" s="34"/>
     </row>
     <row r="31" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3602,25 +3588,25 @@
       <c r="I31" s="29"/>
       <c r="J31" s="38"/>
       <c r="K31" s="39"/>
-      <c r="L31" s="97"/>
-      <c r="M31" s="82"/>
-      <c r="N31" s="79"/>
-      <c r="O31" s="80"/>
-      <c r="P31" s="152"/>
-      <c r="Q31" s="97"/>
-      <c r="R31" s="97"/>
-      <c r="S31" s="97"/>
-      <c r="T31" s="115"/>
-      <c r="U31" s="142"/>
-      <c r="V31" s="80"/>
-      <c r="W31" s="142"/>
-      <c r="X31" s="79"/>
-      <c r="Y31" s="79"/>
-      <c r="Z31" s="79"/>
-      <c r="AA31" s="79"/>
-      <c r="AB31" s="79"/>
-      <c r="AC31" s="79"/>
-      <c r="AD31" s="119"/>
+      <c r="L31" s="103"/>
+      <c r="M31" s="171"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="111"/>
+      <c r="Q31" s="103"/>
+      <c r="R31" s="103"/>
+      <c r="S31" s="103"/>
+      <c r="T31" s="104"/>
+      <c r="U31" s="107"/>
+      <c r="V31" s="94"/>
+      <c r="W31" s="107"/>
+      <c r="X31" s="100"/>
+      <c r="Y31" s="100"/>
+      <c r="Z31" s="100"/>
+      <c r="AA31" s="100"/>
+      <c r="AB31" s="100"/>
+      <c r="AC31" s="100"/>
+      <c r="AD31" s="101"/>
       <c r="AE31" s="34"/>
     </row>
     <row r="32" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3637,27 +3623,27 @@
       <c r="I32" s="29"/>
       <c r="J32" s="35"/>
       <c r="K32" s="29"/>
-      <c r="L32" s="97"/>
-      <c r="M32" s="81"/>
-      <c r="N32" s="83" t="s">
+      <c r="L32" s="103"/>
+      <c r="M32" s="170"/>
+      <c r="N32" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="O32" s="84"/>
-      <c r="P32" s="134"/>
-      <c r="Q32" s="135"/>
-      <c r="R32" s="135"/>
-      <c r="S32" s="135"/>
-      <c r="T32" s="136"/>
-      <c r="U32" s="181"/>
-      <c r="V32" s="172"/>
-      <c r="W32" s="121"/>
-      <c r="X32" s="180"/>
-      <c r="Y32" s="135"/>
-      <c r="Z32" s="135"/>
-      <c r="AA32" s="135"/>
-      <c r="AB32" s="135"/>
-      <c r="AC32" s="135"/>
-      <c r="AD32" s="144"/>
+      <c r="O32" s="93"/>
+      <c r="P32" s="105"/>
+      <c r="Q32" s="98"/>
+      <c r="R32" s="98"/>
+      <c r="S32" s="98"/>
+      <c r="T32" s="106"/>
+      <c r="U32" s="123"/>
+      <c r="V32" s="112"/>
+      <c r="W32" s="113"/>
+      <c r="X32" s="109"/>
+      <c r="Y32" s="98"/>
+      <c r="Z32" s="98"/>
+      <c r="AA32" s="98"/>
+      <c r="AB32" s="98"/>
+      <c r="AC32" s="98"/>
+      <c r="AD32" s="99"/>
       <c r="AE32" s="34"/>
     </row>
     <row r="33" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3674,25 +3660,25 @@
       <c r="I33" s="29"/>
       <c r="J33" s="35"/>
       <c r="K33" s="39"/>
-      <c r="L33" s="97"/>
-      <c r="M33" s="82"/>
-      <c r="N33" s="79"/>
-      <c r="O33" s="80"/>
-      <c r="P33" s="116"/>
-      <c r="Q33" s="79"/>
-      <c r="R33" s="79"/>
-      <c r="S33" s="79"/>
-      <c r="T33" s="80"/>
-      <c r="U33" s="142"/>
-      <c r="V33" s="80"/>
-      <c r="W33" s="142"/>
-      <c r="X33" s="79"/>
-      <c r="Y33" s="79"/>
-      <c r="Z33" s="79"/>
-      <c r="AA33" s="79"/>
-      <c r="AB33" s="79"/>
-      <c r="AC33" s="79"/>
-      <c r="AD33" s="119"/>
+      <c r="L33" s="103"/>
+      <c r="M33" s="171"/>
+      <c r="N33" s="100"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="96"/>
+      <c r="Q33" s="100"/>
+      <c r="R33" s="100"/>
+      <c r="S33" s="100"/>
+      <c r="T33" s="94"/>
+      <c r="U33" s="107"/>
+      <c r="V33" s="94"/>
+      <c r="W33" s="107"/>
+      <c r="X33" s="100"/>
+      <c r="Y33" s="100"/>
+      <c r="Z33" s="100"/>
+      <c r="AA33" s="100"/>
+      <c r="AB33" s="100"/>
+      <c r="AC33" s="100"/>
+      <c r="AD33" s="101"/>
       <c r="AE33" s="34"/>
     </row>
     <row r="34" spans="1:31" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -3709,27 +3695,27 @@
       <c r="I34" s="37"/>
       <c r="J34" s="35"/>
       <c r="K34" s="29"/>
-      <c r="L34" s="97"/>
-      <c r="M34" s="85"/>
-      <c r="N34" s="87" t="s">
+      <c r="L34" s="103"/>
+      <c r="M34" s="224"/>
+      <c r="N34" s="226" t="s">
         <v>32</v>
       </c>
-      <c r="O34" s="89"/>
-      <c r="P34" s="173"/>
-      <c r="Q34" s="135"/>
-      <c r="R34" s="135"/>
-      <c r="S34" s="135"/>
-      <c r="T34" s="136"/>
-      <c r="U34" s="173"/>
-      <c r="V34" s="175"/>
-      <c r="W34" s="176"/>
-      <c r="X34" s="177"/>
-      <c r="Y34" s="135"/>
-      <c r="Z34" s="135"/>
-      <c r="AA34" s="135"/>
-      <c r="AB34" s="135"/>
-      <c r="AC34" s="135"/>
-      <c r="AD34" s="144"/>
+      <c r="O34" s="227"/>
+      <c r="P34" s="114"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="98"/>
+      <c r="S34" s="98"/>
+      <c r="T34" s="106"/>
+      <c r="U34" s="114"/>
+      <c r="V34" s="119"/>
+      <c r="W34" s="120"/>
+      <c r="X34" s="121"/>
+      <c r="Y34" s="98"/>
+      <c r="Z34" s="98"/>
+      <c r="AA34" s="98"/>
+      <c r="AB34" s="98"/>
+      <c r="AC34" s="98"/>
+      <c r="AD34" s="99"/>
       <c r="AE34" s="34"/>
     </row>
     <row r="35" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3746,25 +3732,25 @@
       <c r="I35" s="49"/>
       <c r="J35" s="50"/>
       <c r="K35" s="51"/>
-      <c r="L35" s="88"/>
-      <c r="M35" s="86"/>
-      <c r="N35" s="88"/>
-      <c r="O35" s="90"/>
-      <c r="P35" s="153"/>
-      <c r="Q35" s="88"/>
-      <c r="R35" s="88"/>
-      <c r="S35" s="88"/>
-      <c r="T35" s="90"/>
-      <c r="U35" s="174"/>
-      <c r="V35" s="90"/>
-      <c r="W35" s="174"/>
-      <c r="X35" s="88"/>
-      <c r="Y35" s="88"/>
-      <c r="Z35" s="88"/>
-      <c r="AA35" s="88"/>
-      <c r="AB35" s="88"/>
-      <c r="AC35" s="88"/>
-      <c r="AD35" s="154"/>
+      <c r="L35" s="116"/>
+      <c r="M35" s="225"/>
+      <c r="N35" s="116"/>
+      <c r="O35" s="117"/>
+      <c r="P35" s="115"/>
+      <c r="Q35" s="116"/>
+      <c r="R35" s="116"/>
+      <c r="S35" s="116"/>
+      <c r="T35" s="117"/>
+      <c r="U35" s="118"/>
+      <c r="V35" s="117"/>
+      <c r="W35" s="118"/>
+      <c r="X35" s="116"/>
+      <c r="Y35" s="116"/>
+      <c r="Z35" s="116"/>
+      <c r="AA35" s="116"/>
+      <c r="AB35" s="116"/>
+      <c r="AC35" s="116"/>
+      <c r="AD35" s="122"/>
       <c r="AE35" s="34"/>
     </row>
     <row r="36" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3802,18 +3788,18 @@
     </row>
     <row r="37" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
-      <c r="B37" s="197" t="s">
+      <c r="B37" s="233" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="198"/>
-      <c r="D37" s="198"/>
-      <c r="E37" s="198"/>
-      <c r="F37" s="198"/>
-      <c r="G37" s="198"/>
-      <c r="H37" s="198"/>
-      <c r="I37" s="198"/>
-      <c r="J37" s="199"/>
-      <c r="K37" s="190"/>
+      <c r="C37" s="234"/>
+      <c r="D37" s="234"/>
+      <c r="E37" s="234"/>
+      <c r="F37" s="234"/>
+      <c r="G37" s="234"/>
+      <c r="H37" s="234"/>
+      <c r="I37" s="234"/>
+      <c r="J37" s="235"/>
+      <c r="K37" s="80"/>
       <c r="L37" s="52"/>
       <c r="M37" s="52"/>
       <c r="N37" s="52"/>
@@ -3831,16 +3817,16 @@
     </row>
     <row r="38" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
-      <c r="B38" s="200"/>
-      <c r="C38" s="135"/>
-      <c r="D38" s="135"/>
-      <c r="E38" s="135"/>
-      <c r="F38" s="135"/>
-      <c r="G38" s="135"/>
-      <c r="H38" s="135"/>
-      <c r="I38" s="135"/>
-      <c r="J38" s="201"/>
-      <c r="K38" s="190"/>
+      <c r="B38" s="173"/>
+      <c r="C38" s="98"/>
+      <c r="D38" s="98"/>
+      <c r="E38" s="98"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="98"/>
+      <c r="H38" s="98"/>
+      <c r="I38" s="98"/>
+      <c r="J38" s="174"/>
+      <c r="K38" s="80"/>
       <c r="L38" s="52"/>
       <c r="M38" s="52"/>
       <c r="N38" s="52"/>
@@ -3859,27 +3845,27 @@
     </row>
     <row r="39" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
-      <c r="B39" s="202"/>
-      <c r="C39" s="203"/>
-      <c r="D39" s="203"/>
-      <c r="E39" s="203"/>
-      <c r="F39" s="203"/>
-      <c r="G39" s="203"/>
-      <c r="H39" s="203"/>
-      <c r="I39" s="203"/>
-      <c r="J39" s="204"/>
-      <c r="K39" s="137" t="s">
+      <c r="B39" s="175"/>
+      <c r="C39" s="147"/>
+      <c r="D39" s="147"/>
+      <c r="E39" s="147"/>
+      <c r="F39" s="147"/>
+      <c r="G39" s="147"/>
+      <c r="H39" s="147"/>
+      <c r="I39" s="147"/>
+      <c r="J39" s="176"/>
+      <c r="K39" s="177" t="s">
         <v>39</v>
       </c>
-      <c r="L39" s="138"/>
-      <c r="M39" s="139"/>
-      <c r="N39" s="139"/>
-      <c r="O39" s="139"/>
-      <c r="P39" s="139"/>
-      <c r="Q39" s="139"/>
-      <c r="R39" s="139"/>
-      <c r="S39" s="139"/>
-      <c r="T39" s="140"/>
+      <c r="L39" s="178"/>
+      <c r="M39" s="133"/>
+      <c r="N39" s="133"/>
+      <c r="O39" s="133"/>
+      <c r="P39" s="133"/>
+      <c r="Q39" s="133"/>
+      <c r="R39" s="133"/>
+      <c r="S39" s="133"/>
+      <c r="T39" s="179"/>
       <c r="U39" s="1"/>
       <c r="V39" s="53"/>
       <c r="W39" s="53"/>
@@ -3894,25 +3880,25 @@
     </row>
     <row r="40" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
-      <c r="B40" s="202"/>
-      <c r="C40" s="203"/>
-      <c r="D40" s="203"/>
-      <c r="E40" s="203"/>
-      <c r="F40" s="203"/>
-      <c r="G40" s="203"/>
-      <c r="H40" s="203"/>
-      <c r="I40" s="203"/>
-      <c r="J40" s="204"/>
-      <c r="K40" s="80"/>
-      <c r="L40" s="116"/>
-      <c r="M40" s="79"/>
-      <c r="N40" s="79"/>
-      <c r="O40" s="79"/>
-      <c r="P40" s="79"/>
-      <c r="Q40" s="79"/>
-      <c r="R40" s="79"/>
-      <c r="S40" s="79"/>
-      <c r="T40" s="119"/>
+      <c r="B40" s="175"/>
+      <c r="C40" s="147"/>
+      <c r="D40" s="147"/>
+      <c r="E40" s="147"/>
+      <c r="F40" s="147"/>
+      <c r="G40" s="147"/>
+      <c r="H40" s="147"/>
+      <c r="I40" s="147"/>
+      <c r="J40" s="176"/>
+      <c r="K40" s="94"/>
+      <c r="L40" s="96"/>
+      <c r="M40" s="100"/>
+      <c r="N40" s="100"/>
+      <c r="O40" s="100"/>
+      <c r="P40" s="100"/>
+      <c r="Q40" s="100"/>
+      <c r="R40" s="100"/>
+      <c r="S40" s="100"/>
+      <c r="T40" s="101"/>
       <c r="U40" s="1"/>
       <c r="W40" s="53"/>
       <c r="X40" s="53"/>
@@ -3926,29 +3912,29 @@
     </row>
     <row r="41" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
-      <c r="B41" s="205" t="s">
+      <c r="B41" s="180" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="100"/>
-      <c r="D41" s="100"/>
-      <c r="E41" s="100"/>
-      <c r="F41" s="100"/>
-      <c r="G41" s="100"/>
-      <c r="H41" s="100"/>
-      <c r="I41" s="100"/>
-      <c r="J41" s="206"/>
+      <c r="C41" s="153"/>
+      <c r="D41" s="153"/>
+      <c r="E41" s="153"/>
+      <c r="F41" s="153"/>
+      <c r="G41" s="153"/>
+      <c r="H41" s="153"/>
+      <c r="I41" s="153"/>
+      <c r="J41" s="181"/>
       <c r="K41" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="L41" s="123"/>
-      <c r="M41" s="100"/>
-      <c r="N41" s="100"/>
-      <c r="O41" s="100"/>
-      <c r="P41" s="100"/>
-      <c r="Q41" s="100"/>
-      <c r="R41" s="100"/>
-      <c r="S41" s="100"/>
-      <c r="T41" s="105"/>
+      <c r="L41" s="182"/>
+      <c r="M41" s="153"/>
+      <c r="N41" s="153"/>
+      <c r="O41" s="153"/>
+      <c r="P41" s="153"/>
+      <c r="Q41" s="153"/>
+      <c r="R41" s="153"/>
+      <c r="S41" s="153"/>
+      <c r="T41" s="183"/>
       <c r="U41" s="1"/>
       <c r="W41" s="53"/>
       <c r="X41" s="56"/>
@@ -3962,33 +3948,33 @@
     </row>
     <row r="42" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
-      <c r="B42" s="207" t="s">
+      <c r="B42" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="78" t="s">
+      <c r="C42" s="189" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="80"/>
+      <c r="D42" s="94"/>
       <c r="E42" s="57"/>
-      <c r="F42" s="78" t="s">
+      <c r="F42" s="189" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="79"/>
-      <c r="H42" s="79"/>
-      <c r="I42" s="80"/>
-      <c r="J42" s="208"/>
+      <c r="G42" s="100"/>
+      <c r="H42" s="100"/>
+      <c r="I42" s="94"/>
+      <c r="J42" s="84"/>
       <c r="K42" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="L42" s="123"/>
-      <c r="M42" s="100"/>
-      <c r="N42" s="100"/>
-      <c r="O42" s="100"/>
-      <c r="P42" s="100"/>
-      <c r="Q42" s="100"/>
-      <c r="R42" s="100"/>
-      <c r="S42" s="100"/>
-      <c r="T42" s="105"/>
+      <c r="L42" s="182"/>
+      <c r="M42" s="153"/>
+      <c r="N42" s="153"/>
+      <c r="O42" s="153"/>
+      <c r="P42" s="153"/>
+      <c r="Q42" s="153"/>
+      <c r="R42" s="153"/>
+      <c r="S42" s="153"/>
+      <c r="T42" s="183"/>
       <c r="U42" s="1"/>
       <c r="V42" s="53"/>
       <c r="W42" s="53"/>
@@ -4003,31 +3989,31 @@
     </row>
     <row r="43" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
-      <c r="B43" s="209"/>
-      <c r="C43" s="99" t="s">
+      <c r="B43" s="185"/>
+      <c r="C43" s="187" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="101"/>
+      <c r="D43" s="152"/>
       <c r="E43" s="58"/>
-      <c r="F43" s="99" t="s">
+      <c r="F43" s="187" t="s">
         <v>47</v>
       </c>
-      <c r="G43" s="100"/>
-      <c r="H43" s="100"/>
-      <c r="I43" s="101"/>
-      <c r="J43" s="210"/>
-      <c r="K43" s="191" t="s">
+      <c r="G43" s="153"/>
+      <c r="H43" s="153"/>
+      <c r="I43" s="152"/>
+      <c r="J43" s="85"/>
+      <c r="K43" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="L43" s="123"/>
-      <c r="M43" s="100"/>
-      <c r="N43" s="100"/>
-      <c r="O43" s="100"/>
-      <c r="P43" s="100"/>
-      <c r="Q43" s="100"/>
-      <c r="R43" s="100"/>
-      <c r="S43" s="100"/>
-      <c r="T43" s="105"/>
+      <c r="L43" s="182"/>
+      <c r="M43" s="153"/>
+      <c r="N43" s="153"/>
+      <c r="O43" s="153"/>
+      <c r="P43" s="153"/>
+      <c r="Q43" s="153"/>
+      <c r="R43" s="153"/>
+      <c r="S43" s="153"/>
+      <c r="T43" s="183"/>
       <c r="U43" s="1"/>
       <c r="AB43" s="53"/>
       <c r="AC43" s="53"/>
@@ -4036,31 +4022,31 @@
     </row>
     <row r="44" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
-      <c r="B44" s="209"/>
-      <c r="C44" s="99" t="s">
+      <c r="B44" s="185"/>
+      <c r="C44" s="187" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="101"/>
+      <c r="D44" s="152"/>
       <c r="E44" s="58"/>
-      <c r="F44" s="102" t="s">
+      <c r="F44" s="188" t="s">
         <v>50</v>
       </c>
-      <c r="G44" s="100"/>
-      <c r="H44" s="100"/>
-      <c r="I44" s="101"/>
-      <c r="J44" s="210"/>
-      <c r="K44" s="192" t="s">
+      <c r="G44" s="153"/>
+      <c r="H44" s="153"/>
+      <c r="I44" s="152"/>
+      <c r="J44" s="85"/>
+      <c r="K44" s="202" t="s">
         <v>51</v>
       </c>
-      <c r="L44" s="186"/>
-      <c r="M44" s="123"/>
-      <c r="N44" s="100"/>
-      <c r="O44" s="100"/>
-      <c r="P44" s="100"/>
-      <c r="Q44" s="100"/>
-      <c r="R44" s="100"/>
-      <c r="S44" s="100"/>
-      <c r="T44" s="105"/>
+      <c r="L44" s="203"/>
+      <c r="M44" s="182"/>
+      <c r="N44" s="153"/>
+      <c r="O44" s="153"/>
+      <c r="P44" s="153"/>
+      <c r="Q44" s="153"/>
+      <c r="R44" s="153"/>
+      <c r="S44" s="153"/>
+      <c r="T44" s="183"/>
       <c r="U44" s="1"/>
       <c r="X44" s="53"/>
       <c r="Y44" s="53"/>
@@ -4073,31 +4059,31 @@
     </row>
     <row r="45" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
-      <c r="B45" s="209"/>
-      <c r="C45" s="102" t="s">
+      <c r="B45" s="185"/>
+      <c r="C45" s="188" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="101"/>
+      <c r="D45" s="152"/>
       <c r="E45" s="58"/>
-      <c r="F45" s="99" t="s">
+      <c r="F45" s="187" t="s">
         <v>53</v>
       </c>
-      <c r="G45" s="100"/>
-      <c r="H45" s="100"/>
-      <c r="I45" s="101"/>
-      <c r="J45" s="210"/>
-      <c r="K45" s="192" t="s">
+      <c r="G45" s="153"/>
+      <c r="H45" s="153"/>
+      <c r="I45" s="152"/>
+      <c r="J45" s="85"/>
+      <c r="K45" s="202" t="s">
         <v>54</v>
       </c>
-      <c r="L45" s="186"/>
-      <c r="M45" s="124"/>
-      <c r="N45" s="125"/>
-      <c r="O45" s="125"/>
-      <c r="P45" s="125"/>
-      <c r="Q45" s="125"/>
-      <c r="R45" s="125"/>
-      <c r="S45" s="125"/>
-      <c r="T45" s="126"/>
+      <c r="L45" s="203"/>
+      <c r="M45" s="190"/>
+      <c r="N45" s="191"/>
+      <c r="O45" s="191"/>
+      <c r="P45" s="191"/>
+      <c r="Q45" s="191"/>
+      <c r="R45" s="191"/>
+      <c r="S45" s="191"/>
+      <c r="T45" s="192"/>
       <c r="U45" s="1"/>
       <c r="AB45" s="53"/>
       <c r="AC45" s="53"/>
@@ -4106,39 +4092,39 @@
     </row>
     <row r="46" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
-      <c r="B46" s="209"/>
-      <c r="C46" s="99" t="s">
+      <c r="B46" s="185"/>
+      <c r="C46" s="187" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="101"/>
+      <c r="D46" s="152"/>
       <c r="E46" s="58"/>
-      <c r="F46" s="102" t="s">
+      <c r="F46" s="188" t="s">
         <v>56</v>
       </c>
-      <c r="G46" s="100"/>
-      <c r="H46" s="100"/>
-      <c r="I46" s="101"/>
-      <c r="J46" s="210"/>
-      <c r="K46" s="193" t="s">
+      <c r="G46" s="153"/>
+      <c r="H46" s="153"/>
+      <c r="I46" s="152"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="215" t="s">
         <v>57</v>
       </c>
-      <c r="L46" s="189"/>
+      <c r="L46" s="216"/>
       <c r="M46" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="N46" s="184"/>
+      <c r="N46" s="78"/>
       <c r="O46" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="P46" s="184"/>
+      <c r="P46" s="78"/>
       <c r="Q46" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="R46" s="184"/>
+      <c r="R46" s="78"/>
       <c r="S46" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="T46" s="185"/>
+      <c r="T46" s="79"/>
       <c r="U46" s="1"/>
       <c r="AB46" s="53"/>
       <c r="AC46" s="53"/>
@@ -4147,25 +4133,25 @@
     </row>
     <row r="47" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
-      <c r="B47" s="209"/>
-      <c r="C47" s="102" t="s">
+      <c r="B47" s="185"/>
+      <c r="C47" s="188" t="s">
         <v>62</v>
       </c>
-      <c r="D47" s="101"/>
+      <c r="D47" s="152"/>
       <c r="E47" s="58"/>
-      <c r="F47" s="102" t="s">
+      <c r="F47" s="188" t="s">
         <v>63</v>
       </c>
-      <c r="G47" s="100"/>
-      <c r="H47" s="100"/>
-      <c r="I47" s="101"/>
-      <c r="J47" s="210"/>
-      <c r="K47" s="192" t="s">
+      <c r="G47" s="153"/>
+      <c r="H47" s="153"/>
+      <c r="I47" s="152"/>
+      <c r="J47" s="85"/>
+      <c r="K47" s="202" t="s">
         <v>77</v>
       </c>
-      <c r="L47" s="187"/>
-      <c r="M47" s="187"/>
-      <c r="N47" s="188"/>
+      <c r="L47" s="217"/>
+      <c r="M47" s="217"/>
+      <c r="N47" s="218"/>
       <c r="O47" s="58"/>
       <c r="P47" s="58" t="s">
         <v>64</v>
@@ -4186,33 +4172,33 @@
     </row>
     <row r="48" spans="1:31" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
-      <c r="B48" s="211"/>
-      <c r="C48" s="212" t="s">
+      <c r="B48" s="186"/>
+      <c r="C48" s="220" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="213"/>
-      <c r="E48" s="214"/>
-      <c r="F48" s="215" t="s">
+      <c r="D48" s="221"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="222" t="s">
         <v>66</v>
       </c>
-      <c r="G48" s="216"/>
-      <c r="H48" s="216"/>
-      <c r="I48" s="213"/>
-      <c r="J48" s="217"/>
-      <c r="K48" s="194" t="s">
+      <c r="G48" s="223"/>
+      <c r="H48" s="223"/>
+      <c r="I48" s="221"/>
+      <c r="J48" s="87"/>
+      <c r="K48" s="219" t="s">
         <v>67</v>
       </c>
-      <c r="L48" s="103"/>
-      <c r="M48" s="127" t="s">
+      <c r="L48" s="207"/>
+      <c r="M48" s="193" t="s">
         <v>68</v>
       </c>
-      <c r="N48" s="107"/>
-      <c r="O48" s="107"/>
-      <c r="P48" s="107"/>
-      <c r="Q48" s="107"/>
-      <c r="R48" s="107"/>
-      <c r="S48" s="107"/>
-      <c r="T48" s="112"/>
+      <c r="N48" s="194"/>
+      <c r="O48" s="194"/>
+      <c r="P48" s="194"/>
+      <c r="Q48" s="194"/>
+      <c r="R48" s="194"/>
+      <c r="S48" s="194"/>
+      <c r="T48" s="195"/>
       <c r="U48" s="1"/>
       <c r="AB48" s="53"/>
       <c r="AC48" s="53"/>
@@ -4221,27 +4207,27 @@
     </row>
     <row r="49" spans="1:31" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
-      <c r="B49" s="195"/>
-      <c r="C49" s="195"/>
-      <c r="D49" s="195"/>
-      <c r="E49" s="196"/>
-      <c r="F49" s="196"/>
-      <c r="G49" s="196"/>
-      <c r="H49" s="196"/>
-      <c r="I49" s="196"/>
-      <c r="J49" s="196"/>
-      <c r="K49" s="128" t="s">
+      <c r="B49" s="82"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="83"/>
+      <c r="G49" s="83"/>
+      <c r="H49" s="83"/>
+      <c r="I49" s="83"/>
+      <c r="J49" s="83"/>
+      <c r="K49" s="196" t="s">
         <v>69</v>
       </c>
-      <c r="L49" s="129"/>
-      <c r="M49" s="129"/>
-      <c r="N49" s="129"/>
-      <c r="O49" s="129"/>
-      <c r="P49" s="129"/>
-      <c r="Q49" s="129"/>
-      <c r="R49" s="129"/>
-      <c r="S49" s="129"/>
-      <c r="T49" s="130"/>
+      <c r="L49" s="197"/>
+      <c r="M49" s="197"/>
+      <c r="N49" s="197"/>
+      <c r="O49" s="197"/>
+      <c r="P49" s="197"/>
+      <c r="Q49" s="197"/>
+      <c r="R49" s="197"/>
+      <c r="S49" s="197"/>
+      <c r="T49" s="198"/>
       <c r="U49" s="1"/>
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
@@ -4259,24 +4245,24 @@
       <c r="H50" s="61"/>
       <c r="I50" s="61"/>
       <c r="J50" s="53"/>
-      <c r="K50" s="131" t="s">
+      <c r="K50" s="199" t="s">
         <v>70</v>
       </c>
-      <c r="L50" s="133" t="s">
+      <c r="L50" s="201" t="s">
         <v>71</v>
       </c>
-      <c r="M50" s="115"/>
-      <c r="N50" s="114" t="s">
+      <c r="M50" s="104"/>
+      <c r="N50" s="211" t="s">
         <v>72</v>
       </c>
-      <c r="O50" s="97"/>
-      <c r="P50" s="115"/>
-      <c r="Q50" s="117" t="s">
+      <c r="O50" s="103"/>
+      <c r="P50" s="104"/>
+      <c r="Q50" s="212" t="s">
         <v>74</v>
       </c>
-      <c r="R50" s="97"/>
-      <c r="S50" s="97"/>
-      <c r="T50" s="118"/>
+      <c r="R50" s="103"/>
+      <c r="S50" s="103"/>
+      <c r="T50" s="128"/>
       <c r="U50" s="1"/>
       <c r="AB50" s="1"/>
       <c r="AC50" s="1"/>
@@ -4294,16 +4280,16 @@
       <c r="H51" s="61"/>
       <c r="I51" s="61"/>
       <c r="J51" s="53"/>
-      <c r="K51" s="132"/>
-      <c r="L51" s="116"/>
-      <c r="M51" s="80"/>
-      <c r="N51" s="116"/>
-      <c r="O51" s="79"/>
-      <c r="P51" s="80"/>
-      <c r="Q51" s="116"/>
-      <c r="R51" s="79"/>
-      <c r="S51" s="79"/>
-      <c r="T51" s="119"/>
+      <c r="K51" s="200"/>
+      <c r="L51" s="96"/>
+      <c r="M51" s="94"/>
+      <c r="N51" s="96"/>
+      <c r="O51" s="100"/>
+      <c r="P51" s="94"/>
+      <c r="Q51" s="96"/>
+      <c r="R51" s="100"/>
+      <c r="S51" s="100"/>
+      <c r="T51" s="101"/>
       <c r="U51" s="1"/>
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
@@ -4322,15 +4308,15 @@
       <c r="I52" s="61"/>
       <c r="J52" s="53"/>
       <c r="K52" s="62"/>
-      <c r="L52" s="120"/>
-      <c r="M52" s="101"/>
-      <c r="N52" s="121"/>
-      <c r="O52" s="100"/>
-      <c r="P52" s="101"/>
-      <c r="Q52" s="104"/>
-      <c r="R52" s="100"/>
-      <c r="S52" s="100"/>
-      <c r="T52" s="105"/>
+      <c r="L52" s="213"/>
+      <c r="M52" s="152"/>
+      <c r="N52" s="113"/>
+      <c r="O52" s="153"/>
+      <c r="P52" s="152"/>
+      <c r="Q52" s="205"/>
+      <c r="R52" s="153"/>
+      <c r="S52" s="153"/>
+      <c r="T52" s="183"/>
       <c r="U52" s="1"/>
       <c r="AB52" s="1"/>
       <c r="AC52" s="1"/>
@@ -4349,15 +4335,15 @@
       <c r="I53" s="61"/>
       <c r="J53" s="53"/>
       <c r="K53" s="62"/>
-      <c r="L53" s="120"/>
-      <c r="M53" s="101"/>
-      <c r="N53" s="122"/>
-      <c r="O53" s="100"/>
-      <c r="P53" s="101"/>
-      <c r="Q53" s="104"/>
-      <c r="R53" s="100"/>
-      <c r="S53" s="100"/>
-      <c r="T53" s="105"/>
+      <c r="L53" s="213"/>
+      <c r="M53" s="152"/>
+      <c r="N53" s="214"/>
+      <c r="O53" s="153"/>
+      <c r="P53" s="152"/>
+      <c r="Q53" s="205"/>
+      <c r="R53" s="153"/>
+      <c r="S53" s="153"/>
+      <c r="T53" s="183"/>
       <c r="U53" s="1"/>
       <c r="AB53" s="1"/>
       <c r="AC53" s="1"/>
@@ -4376,15 +4362,15 @@
       <c r="I54" s="61"/>
       <c r="J54" s="53"/>
       <c r="K54" s="62"/>
-      <c r="L54" s="120"/>
-      <c r="M54" s="101"/>
-      <c r="N54" s="99"/>
-      <c r="O54" s="100"/>
-      <c r="P54" s="101"/>
-      <c r="Q54" s="104"/>
-      <c r="R54" s="100"/>
-      <c r="S54" s="100"/>
-      <c r="T54" s="105"/>
+      <c r="L54" s="213"/>
+      <c r="M54" s="152"/>
+      <c r="N54" s="187"/>
+      <c r="O54" s="153"/>
+      <c r="P54" s="152"/>
+      <c r="Q54" s="205"/>
+      <c r="R54" s="153"/>
+      <c r="S54" s="153"/>
+      <c r="T54" s="183"/>
       <c r="U54" s="1"/>
       <c r="AB54" s="1"/>
       <c r="AC54" s="1"/>
@@ -4403,15 +4389,15 @@
       <c r="I55" s="61"/>
       <c r="J55" s="53"/>
       <c r="K55" s="62"/>
-      <c r="L55" s="108"/>
-      <c r="M55" s="101"/>
-      <c r="N55" s="99"/>
-      <c r="O55" s="100"/>
-      <c r="P55" s="101"/>
-      <c r="Q55" s="104"/>
-      <c r="R55" s="100"/>
-      <c r="S55" s="100"/>
-      <c r="T55" s="105"/>
+      <c r="L55" s="204"/>
+      <c r="M55" s="152"/>
+      <c r="N55" s="187"/>
+      <c r="O55" s="153"/>
+      <c r="P55" s="152"/>
+      <c r="Q55" s="205"/>
+      <c r="R55" s="153"/>
+      <c r="S55" s="153"/>
+      <c r="T55" s="183"/>
       <c r="U55" s="1"/>
       <c r="AB55" s="1"/>
       <c r="AC55" s="1"/>
@@ -4430,15 +4416,15 @@
       <c r="I56" s="53"/>
       <c r="J56" s="53"/>
       <c r="K56" s="64"/>
-      <c r="L56" s="109"/>
-      <c r="M56" s="103"/>
-      <c r="N56" s="110"/>
-      <c r="O56" s="107"/>
-      <c r="P56" s="103"/>
-      <c r="Q56" s="111"/>
-      <c r="R56" s="107"/>
-      <c r="S56" s="107"/>
-      <c r="T56" s="112"/>
+      <c r="L56" s="206"/>
+      <c r="M56" s="207"/>
+      <c r="N56" s="208"/>
+      <c r="O56" s="194"/>
+      <c r="P56" s="207"/>
+      <c r="Q56" s="209"/>
+      <c r="R56" s="194"/>
+      <c r="S56" s="194"/>
+      <c r="T56" s="195"/>
       <c r="U56" s="1"/>
       <c r="AB56" s="1"/>
       <c r="AC56" s="1"/>
@@ -4454,8 +4440,8 @@
       <c r="F57" s="65"/>
       <c r="G57" s="65"/>
       <c r="H57" s="66"/>
-      <c r="I57" s="113"/>
-      <c r="J57" s="97"/>
+      <c r="I57" s="210"/>
+      <c r="J57" s="103"/>
       <c r="K57" s="66"/>
       <c r="L57" s="67"/>
       <c r="M57" s="67"/>
@@ -10596,63 +10582,108 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="187">
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="X16:AD17"/>
-    <mergeCell ref="P12:T13"/>
-    <mergeCell ref="P14:T15"/>
-    <mergeCell ref="U14:U15"/>
-    <mergeCell ref="V14:V15"/>
-    <mergeCell ref="W14:W15"/>
-    <mergeCell ref="P16:T17"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="P18:T19"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="V18:V19"/>
-    <mergeCell ref="W18:W19"/>
-    <mergeCell ref="X18:AD19"/>
-    <mergeCell ref="P20:T21"/>
-    <mergeCell ref="U20:U21"/>
-    <mergeCell ref="X20:AD21"/>
-    <mergeCell ref="V20:V21"/>
-    <mergeCell ref="W20:W21"/>
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="V22:V23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:AD23"/>
-    <mergeCell ref="P24:T25"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="V24:V25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:AD25"/>
-    <mergeCell ref="U26:U27"/>
-    <mergeCell ref="X26:AD27"/>
-    <mergeCell ref="V26:V27"/>
-    <mergeCell ref="W26:W27"/>
-    <mergeCell ref="P28:T29"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="V28:V29"/>
-    <mergeCell ref="W28:W29"/>
-    <mergeCell ref="X28:AD29"/>
-    <mergeCell ref="V32:V33"/>
-    <mergeCell ref="W32:W33"/>
-    <mergeCell ref="P34:T35"/>
-    <mergeCell ref="U34:U35"/>
-    <mergeCell ref="V34:V35"/>
-    <mergeCell ref="W34:W35"/>
-    <mergeCell ref="X34:AD35"/>
-    <mergeCell ref="P30:T31"/>
-    <mergeCell ref="U30:U31"/>
-    <mergeCell ref="V30:V31"/>
-    <mergeCell ref="W30:W31"/>
-    <mergeCell ref="X30:AD31"/>
-    <mergeCell ref="P32:T33"/>
-    <mergeCell ref="U32:U33"/>
-    <mergeCell ref="X32:AD33"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="N32:N33"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="O34:O35"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:L35"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="N54:P54"/>
+    <mergeCell ref="Q54:T54"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="L55:M55"/>
+    <mergeCell ref="N55:P55"/>
+    <mergeCell ref="Q55:T55"/>
+    <mergeCell ref="L56:M56"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="Q56:T56"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="N50:P51"/>
+    <mergeCell ref="Q50:T51"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="N52:P52"/>
+    <mergeCell ref="Q52:T52"/>
+    <mergeCell ref="L53:M53"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="Q53:T53"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="M44:T44"/>
+    <mergeCell ref="M45:T45"/>
+    <mergeCell ref="M48:T48"/>
+    <mergeCell ref="K49:T49"/>
+    <mergeCell ref="K50:K51"/>
+    <mergeCell ref="L50:M51"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="P22:T23"/>
+    <mergeCell ref="B38:J40"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L39:T40"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="L41:T41"/>
+    <mergeCell ref="L42:T42"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="P26:T27"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="L43:T43"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="P10:T11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="W12:W13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O15"/>
     <mergeCell ref="W2:AD2"/>
     <mergeCell ref="W3:AD8"/>
     <mergeCell ref="X10:AD11"/>
@@ -10677,149 +10708,104 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="U8:V8"/>
     <mergeCell ref="M9:AD9"/>
+    <mergeCell ref="V32:V33"/>
+    <mergeCell ref="W32:W33"/>
+    <mergeCell ref="P34:T35"/>
+    <mergeCell ref="U34:U35"/>
+    <mergeCell ref="V34:V35"/>
+    <mergeCell ref="W34:W35"/>
+    <mergeCell ref="X34:AD35"/>
+    <mergeCell ref="P30:T31"/>
+    <mergeCell ref="U30:U31"/>
+    <mergeCell ref="V30:V31"/>
+    <mergeCell ref="W30:W31"/>
+    <mergeCell ref="X30:AD31"/>
+    <mergeCell ref="P32:T33"/>
+    <mergeCell ref="U32:U33"/>
+    <mergeCell ref="X32:AD33"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="X26:AD27"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="W26:W27"/>
+    <mergeCell ref="P28:T29"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="V28:V29"/>
+    <mergeCell ref="W28:W29"/>
+    <mergeCell ref="X28:AD29"/>
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="V22:V23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:AD23"/>
+    <mergeCell ref="P24:T25"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="V24:V25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:AD25"/>
+    <mergeCell ref="P18:T19"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="V18:V19"/>
+    <mergeCell ref="W18:W19"/>
+    <mergeCell ref="X18:AD19"/>
+    <mergeCell ref="P20:T21"/>
+    <mergeCell ref="U20:U21"/>
+    <mergeCell ref="X20:AD21"/>
+    <mergeCell ref="V20:V21"/>
+    <mergeCell ref="W20:W21"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="X16:AD17"/>
+    <mergeCell ref="P12:T13"/>
+    <mergeCell ref="P14:T15"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="V14:V15"/>
+    <mergeCell ref="W14:W15"/>
+    <mergeCell ref="P16:T17"/>
+    <mergeCell ref="U16:U17"/>
     <mergeCell ref="U12:U13"/>
     <mergeCell ref="V12:V13"/>
     <mergeCell ref="X12:AD13"/>
     <mergeCell ref="X14:AD15"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="P10:T11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="W12:W13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="B38:J40"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L39:T40"/>
-    <mergeCell ref="B41:J41"/>
-    <mergeCell ref="L41:T41"/>
-    <mergeCell ref="L42:T42"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="P26:T27"/>
-    <mergeCell ref="B42:B48"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="L43:T43"/>
-    <mergeCell ref="M44:T44"/>
-    <mergeCell ref="M45:T45"/>
-    <mergeCell ref="M48:T48"/>
-    <mergeCell ref="K49:T49"/>
-    <mergeCell ref="K50:K51"/>
-    <mergeCell ref="L50:M51"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="P22:T23"/>
-    <mergeCell ref="L55:M55"/>
-    <mergeCell ref="N55:P55"/>
-    <mergeCell ref="Q55:T55"/>
-    <mergeCell ref="L56:M56"/>
-    <mergeCell ref="N56:P56"/>
-    <mergeCell ref="Q56:T56"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="N50:P51"/>
-    <mergeCell ref="Q50:T51"/>
-    <mergeCell ref="L52:M52"/>
-    <mergeCell ref="N52:P52"/>
-    <mergeCell ref="Q52:T52"/>
-    <mergeCell ref="L53:M53"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="Q53:T53"/>
-    <mergeCell ref="L54:M54"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="N54:P54"/>
-    <mergeCell ref="Q54:T54"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="N32:N33"/>
-    <mergeCell ref="O32:O33"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="N34:N35"/>
-    <mergeCell ref="O34:O35"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:L35"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="B37:J37"/>
   </mergeCells>
   <conditionalFormatting sqref="E42:E48">
-    <cfRule type="containsBlanks" dxfId="7" priority="6">
+    <cfRule type="containsBlanks" dxfId="6" priority="6">
       <formula>LEN(TRIM(E42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42:J48">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(J42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:T6">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(J3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39:T43">
-    <cfRule type="containsBlanks" dxfId="4" priority="2">
+    <cfRule type="containsBlanks" dxfId="3" priority="2">
       <formula>LEN(TRIM(L39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44:T45">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(M44))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M48:T48">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(M48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46 P46 R46 T46">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>NOT(OR($N46,$P46,$R46,$T46))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="15">
+  <dataValidations count="25">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L42" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Clear,Few (&lt; ¼ of sky),Scattered (¼ - ½ of sky),Broken
 (&gt; ½ of sky),Overcast
@@ -10847,9 +10833,6 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L41" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"None,Rain,Snow,Graupel,Hail"</formula1>
     </dataValidation>
-    <dataValidation type="custom" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="H3" xr:uid="{00000000-0002-0000-0000-000008000000}">
-      <formula1>OR(NOT(ISERROR(DATEVALUE(H3))), AND(ISNUMBER(H3), LEFT(CELL("format", H3))="D"))</formula1>
-    </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L43" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"Calm,Light,Moderate,Strong,Extreme"</formula1>
     </dataValidation>
@@ -10868,6 +10851,17 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="U12:U35" xr:uid="{3B0FAC7B-A561-044C-ADE1-C03ED8F6BEB4}">
       <formula1>"SH,PP,PPgp,DF,RG,FC,MF,MFcr,IF, FCsf"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Location" prompt="General area of work, e.g. Central Sierra Snow Lab, Grand Mesa, East River Watershed" sqref="B3:G4" xr:uid="{8DFD6608-A2C6-984F-BBF0-AF9227C114CF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Site" prompt="two word site name, e.g. East Open, Banner Summit, North Trees" sqref="B6:G6" xr:uid="{1400458B-15A4-8E43-B6BD-54D20C8F385E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Pit ID" prompt="2-letter state, 2-letter location, 2-letter site, e.g CA-California, SL-Central Sierra Snow Lab, North Trees-NT = CASLNT_x000a__x000a_+ date string (e.g. 20250101)_x000a_" sqref="B8:E8" xr:uid="{FBCBDB8C-F615-F142-AA0D-E1B280B9E82B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Height of Snow (HS)" prompt="enter the snow pit height (e.g 158)" sqref="F8:G8" xr:uid="{BE16D183-4D62-D042-BE62-C23AF79930C9}"/>
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" promptTitle="Date" prompt="yyyy-mm-dd" sqref="H3:I4" xr:uid="{2FD0BCE3-C9D3-9C42-8089-CCB216C215E7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time" prompt="Military, HH:MM" sqref="H6:I6" xr:uid="{FF1BBA4A-76A8-EB4F-9B02-36E39E60311C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Liquid Water Content sensor " prompt="record instrument serial number" sqref="H8:I8" xr:uid="{F8380F51-7F0D-F94B-BA5C-C2639F662449}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Easting" prompt="enter values only, no letters" sqref="J8:M8" xr:uid="{5DC37F26-C640-B440-ACAE-40F4084EB14E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Northing" prompt="enter values only, no letters" sqref="N8:R8" xr:uid="{DEE65961-52D7-4A42-9A1D-AE7ACBD66715}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Observer" prompt="First initial and last name (e.g. M. Mason). For a list separate with a comma." sqref="J3:T6" xr:uid="{E9C991E2-2F07-9C42-8FC7-D9AB73F3D74D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Zone" prompt="enter the UTM zone, 2-digit number, no letters" sqref="S8:T8" xr:uid="{B7842707-5800-A743-A9AE-DA70020D9AD3}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>